<commit_message>
fix: Reparar Interoperabilidad y Validar Flujo ETL
Este parche corrige una serie de errores críticos que impedían la comunicación entre el frontend y el backend.

- Se actualizó el contrato de la API (`openapi.yaml`) para que coincidiera con la implementación real del backend.
- Se regeneró el cliente de la API del frontend y se configuró la URL base correcta.
- Se corrigieron errores de enrutamiento y se ajustó la política de CORS.
- Se actualizaron las dependencias de `langchain-google-genai` para resolver un conflicto con la API de Gemini.
- Se incluye un script de prueba (`smoke_test.sh`) y los datos necesarios para verificar de forma automática y completa el flujo ETL, desde la creación de la sesión hasta la respuesta del agente de IA.
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Ventas" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,27 +436,27 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>Producto</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>value</t>
+          <t>Ventas</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>test1</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -465,14 +465,27 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>test2</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C3" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>7</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>200</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: Corregir lógica de inyección de contexto en el agente LLM
Implementa la corrección para el manejo del contexto del agente LLM. El endpoint del chat ahora construye un prompt estructurado utilizando los mensajes de Sistema y Humano de LangChain, asegurando que el contexto del DataFrame se pase correctamente al modelo.

- Refactorizado `backend/agent/api.py` para usar `SystemMessage` y `HumanMessage`.
- Modificado `backend/llm/llm_router.py` para aceptar una lista de mensajes.
- Añadida la dependencia `tabulate` para el formateo de datos en Markdown.

Nota: La verificación final de esta corrección está bloqueada por un conflicto de dependencias irresoluble entre `langchain` y `langchain-experimental`. Se recomienda una revisión de `requirements.in` como tarea de seguimiento.
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Ventas" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,27 +436,27 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>Producto</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>value</t>
+          <t>Ventas</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>test1</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -465,14 +465,27 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>test2</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C3" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>7</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>200</v>
       </c>
     </row>

</xml_diff>